<commit_message>
accueil + joli et réflexion sur l'inscription
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\covoiturage\covoiturage\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
@@ -133,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +173,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,12 +212,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -231,9 +237,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,12 +250,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -291,7 +300,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,7 +335,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -537,11 +546,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="59.85546875" customWidth="1"/>
@@ -750,40 +759,40 @@
       <c r="AA5" s="3"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="AA6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="AA6" s="10"/>
     </row>
     <row r="7" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="11"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -809,6 +818,7 @@
       <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
@@ -952,7 +962,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -964,7 +974,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
supprimer des trajets fait
A noter que c'est pas du tout parfait. En effet, le trajet ne se
supprime pas si des gens y sont inscrit. Je préfèrerais donc ajouter un
champs binaire au trajet indiquant si le trajet est visible ou non.
Sinon on devrait supprime par cascade les enregistrements ou mettre à
null le ride_fk, on devrait supprimer également les votes. Je pense que
c'est pas une bonne idée. Je souhaite donc ajouter une visibilité. ça
pourrait être utile également pour une raison d'historique
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -547,7 +547,7 @@
   <dimension ref="A2:AB35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="H8" s="10"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -806,12 +806,14 @@
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>

</xml_diff>

<commit_message>
syncro avec elliott ?
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -547,7 +547,7 @@
   <dimension ref="A2:AB35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,14 +793,13 @@
         <v>4</v>
       </c>
       <c r="H8" s="10"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>

</xml_diff>

<commit_message>
Revert "syncro avec elliott ?"
This reverts commit e143d6887a02d2eabaca18287e31efa45f669650.
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -547,7 +547,7 @@
   <dimension ref="A2:AB35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,13 +793,14 @@
         <v>4</v>
       </c>
       <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>

</xml_diff>